<commit_message>
Simple neuron with weights, bias and activation (sigmoid) in Excel
Signed-off-by: syedmeesamali <syedmeesamali@yahoo.com>
</commit_message>
<xml_diff>
--- a/9_Machine_learning/1_Neural/Neurons/Neural Network.xlsx
+++ b/9_Machine_learning/1_Neural/Neurons/Neural Network.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Repos\Python\9_Machine_learning\1_Neural\Neurons\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3192382-4EBE-4BFA-826F-9C63F3B96A9D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{703AF94E-E0E3-4946-9FC0-889D64950FA9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>1. Simple Neuron Model</t>
   </si>
@@ -56,9 +56,6 @@
     <t>Output</t>
   </si>
   <si>
-    <t>x1 * w1 + x2 * w2 + b</t>
-  </si>
-  <si>
     <t>Weight - 1</t>
   </si>
   <si>
@@ -72,13 +69,19 @@
   </si>
   <si>
     <t>Input - 2</t>
+  </si>
+  <si>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>f (x1 * w1 + x2 * w2 + b)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -87,13 +90,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -147,8 +143,34 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FFC00000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -191,8 +213,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -215,64 +243,104 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFCCFFCC"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -289,15 +357,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>148828</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:colOff>158353</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>358378</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -312,8 +380,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1777603" y="228600"/>
-          <a:ext cx="3705225" cy="2667000"/>
+          <a:off x="2796778" y="361950"/>
+          <a:ext cx="4394597" cy="3095625"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -336,66 +404,6 @@
         </a:fillRef>
         <a:effectRef idx="2">
           <a:schemeClr val="accent5"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>417909</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>178593</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="Arrow: Right 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E7B4D3B-AB39-463B-B956-692F59746646}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5542359" y="1359693"/>
-          <a:ext cx="1172766" cy="230982"/>
-        </a:xfrm>
-        <a:prstGeom prst="rightArrow">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent2">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent2"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent2"/>
         </a:effectRef>
         <a:fontRef idx="minor">
           <a:schemeClr val="lt1"/>
@@ -472,16 +480,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>495301</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>39289</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>390526</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>105964</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>381001</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>276226</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>158353</xdr:rowOff>
+      <xdr:rowOff>25003</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -496,8 +504,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3790951" y="1029889"/>
-          <a:ext cx="1104900" cy="1071564"/>
+          <a:off x="5915026" y="1315639"/>
+          <a:ext cx="1104900" cy="1119189"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartPunchedTape">
           <a:avLst/>
@@ -646,6 +654,126 @@
         </a:fillRef>
         <a:effectRef idx="3">
           <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>107157</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Arrow: Right 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C82904D5-7CC9-4D4F-8768-FB9D2AFDB884}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7134225" y="1666875"/>
+          <a:ext cx="572691" cy="250032"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>11907</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Arrow: Right 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB56404D-E123-44C7-85EA-9B22B633A2C8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5238750" y="1771650"/>
+          <a:ext cx="447675" cy="250032"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
         </a:effectRef>
         <a:fontRef idx="minor">
           <a:schemeClr val="lt1"/>
@@ -928,148 +1056,175 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:R15"/>
+  <dimension ref="B3:T15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="6.42578125" style="9" customWidth="1"/>
-    <col min="4" max="4" width="7" style="9" customWidth="1"/>
+    <col min="3" max="3" width="6.42578125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="7" style="5" customWidth="1"/>
     <col min="5" max="5" width="13.140625" style="1" customWidth="1"/>
-    <col min="6" max="7" width="7" style="6" customWidth="1"/>
+    <col min="6" max="7" width="7" style="2" customWidth="1"/>
     <col min="8" max="8" width="4.28515625" style="1" customWidth="1"/>
     <col min="9" max="9" width="6.7109375" style="1" customWidth="1"/>
-    <col min="10" max="14" width="9.140625" style="1"/>
-    <col min="15" max="15" width="5.85546875" style="1" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="1"/>
+    <col min="10" max="10" width="6.85546875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="7.5703125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="12.28515625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" style="1"/>
+    <col min="14" max="14" width="6" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:18" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B3" s="5" t="s">
+    <row r="3" spans="2:20" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B3" s="18" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="C6" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="18" t="s">
-        <v>8</v>
-      </c>
+    <row r="6" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="C6" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="16"/>
+      <c r="H6" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="I6" s="17"/>
     </row>
-    <row r="7" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C7" s="19" t="s">
+    <row r="7" spans="2:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C7" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="20">
+      <c r="D7" s="15">
         <v>2</v>
       </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="16" t="s">
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="I7" s="11">
-        <v>1</v>
+      <c r="I7" s="7">
+        <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D8" s="10"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="12"/>
-      <c r="P8" s="2" t="s">
+    <row r="8" spans="2:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D8" s="6"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="8"/>
+      <c r="K8" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="P8" s="19" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D9" s="10"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="I9" s="12"/>
-    </row>
-    <row r="10" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D10" s="10"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="I10" s="14">
-        <v>-1</v>
-      </c>
-      <c r="P10" s="4">
+    <row r="9" spans="2:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D9" s="6"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="I9" s="17"/>
+      <c r="K9" s="20">
         <f>D7*I7+D14*I14+I10</f>
         <v>7</v>
       </c>
-      <c r="R10" s="3" t="s">
-        <v>7</v>
+      <c r="P9" s="22">
+        <f>1/(1-EXP(1)^(-K9))</f>
+        <v>1.0009127142532217</v>
       </c>
     </row>
-    <row r="11" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D11" s="10"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="12"/>
+    <row r="10" spans="2:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D10" s="6"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="I10" s="10">
+        <v>4</v>
+      </c>
+      <c r="K10" s="21"/>
+      <c r="P10" s="23"/>
+      <c r="R10" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="S10" s="25"/>
+      <c r="T10" s="25"/>
     </row>
-    <row r="12" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D12" s="10"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="12"/>
+    <row r="11" spans="2:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D11" s="6"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="8"/>
+      <c r="K11" s="21"/>
+      <c r="P11" s="23"/>
     </row>
-    <row r="13" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C13" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="I13" s="12"/>
+    <row r="12" spans="2:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D12" s="6"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="8"/>
     </row>
-    <row r="14" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C14" s="19" t="s">
+    <row r="13" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="C13" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="16"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="I13" s="17"/>
+    </row>
+    <row r="14" spans="2:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C14" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="20">
+      <c r="D14" s="15">
         <v>3</v>
       </c>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="16" t="s">
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="I14" s="17">
-        <v>2</v>
+      <c r="I14" s="13">
+        <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="H15" s="15"/>
-      <c r="I15" s="15"/>
+    <row r="15" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
     </row>
   </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="P9:P11"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="K9:K11"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
Neurons and neural network basics
Signed-off-by: syedmeesamali <syedmeesamali@yahoo.com>
</commit_message>
<xml_diff>
--- a/9_Machine_learning/1_Neural/Neurons/Neural Network.xlsx
+++ b/9_Machine_learning/1_Neural/Neurons/Neural Network.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Repos\Python\9_Machine_learning\1_Neural\Neurons\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{703AF94E-E0E3-4946-9FC0-889D64950FA9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E4EE60C-FE91-46CE-93C4-0FE2AE301B92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="15">
   <si>
     <t>1. Simple Neuron Model</t>
   </si>
@@ -75,6 +75,9 @@
   </si>
   <si>
     <t>f (x1 * w1 + x2 * w2 + b)</t>
+  </si>
+  <si>
+    <t>2. Simple Neural Network</t>
   </si>
 </sst>
 </file>
@@ -265,7 +268,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -306,20 +309,8 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -330,6 +321,27 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -354,16 +366,72 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1076325" cy="702119"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Picture 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EA9FD2E5-2924-43FA-8251-D249093F4D29}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5181600" y="5276850"/>
+          <a:ext cx="1076325" cy="702119"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>158353</xdr:colOff>
+      <xdr:colOff>158352</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
+      <xdr:colOff>190499</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
@@ -380,8 +448,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2796778" y="361950"/>
-          <a:ext cx="4394597" cy="3095625"/>
+          <a:off x="2796777" y="361950"/>
+          <a:ext cx="4489847" cy="3095625"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -482,14 +550,14 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>390526</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>105964</xdr:rowOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>276226</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>25003</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -504,8 +572,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5915026" y="1315639"/>
-          <a:ext cx="1104900" cy="1119189"/>
+          <a:off x="5657851" y="1171575"/>
+          <a:ext cx="1476374" cy="1571625"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartPunchedTape">
           <a:avLst/>
@@ -533,21 +601,7 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>      f(x)</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>    (Activation      </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>      Function)</a:t>
+            <a:t>[Sigmoid Activation]</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -673,15 +727,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>28575</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>107157</xdr:rowOff>
+      <xdr:rowOff>145257</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -696,8 +750,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7134225" y="1666875"/>
-          <a:ext cx="572691" cy="250032"/>
+          <a:off x="7296150" y="1704975"/>
+          <a:ext cx="438150" cy="250032"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
           <a:avLst/>
@@ -758,6 +812,843 @@
         <a:xfrm>
           <a:off x="5238750" y="1771650"/>
           <a:ext cx="447675" cy="250032"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>63944</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA41562F-A347-42D0-B7B0-54AEF9ADC373}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5724525" y="1771650"/>
+          <a:ext cx="1076325" cy="702119"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>167877</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="Oval 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3E33818-C16F-458C-9FC0-8EC9BE3BDF97}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2806302" y="4295775"/>
+          <a:ext cx="3508773" cy="2524125"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent4">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+            <a:alpha val="30000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="38100"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent5"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent5"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>142874</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>342899</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>100012</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="Arrow: Right 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7B464B91-A2A5-4E55-B244-CAE0C3E2CAF4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5185591">
+          <a:off x="4329112" y="5343524"/>
+          <a:ext cx="438150" cy="200025"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>123903</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>46561</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>166732</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>8461</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="Arrow: Right 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BE9520C6-DA1B-42CD-A90D-CBD86D3C0D7F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="1799063">
+          <a:off x="1886028" y="6790261"/>
+          <a:ext cx="1852579" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="3">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>95252</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>261424</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="Arrow: Right 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{153669C3-FCCB-4769-8FD4-6C4060579A02}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="20726102">
+          <a:off x="1857377" y="6029325"/>
+          <a:ext cx="1042472" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="3">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>145257</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="Arrow: Right 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F32DA659-705A-4B75-80CC-C134C1377832}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6334125" y="5257800"/>
+          <a:ext cx="790575" cy="250032"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>428624</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>47624</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>50007</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="19" name="Arrow: Right 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CBF0B103-A046-4E84-BA34-776D452D23A2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="19611347">
+          <a:off x="4733924" y="5962650"/>
+          <a:ext cx="581025" cy="250032"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1076325" cy="702119"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="27" name="Picture 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3B8260A-6BA1-48A6-9C60-30DF7AB1E6C1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5181600" y="5276850"/>
+          <a:ext cx="1076325" cy="702119"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>167877</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="28" name="Oval 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E16C7DE2-5FAA-446C-91A8-D1D3F097AA97}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2806302" y="4295775"/>
+          <a:ext cx="3508773" cy="2533650"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent4">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+            <a:alpha val="30000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="38100"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent5"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent5"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>142874</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>342899</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>100012</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="29" name="Arrow: Right 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E0483A9F-16DA-4470-8734-A8EA995168C7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5185591">
+          <a:off x="4329112" y="5343524"/>
+          <a:ext cx="438150" cy="200025"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>428624</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>47624</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>50007</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="30" name="Arrow: Right 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20FEB80A-65D5-4001-9DBF-CA92AFAE82D3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="19611347">
+          <a:off x="4733924" y="5962650"/>
+          <a:ext cx="581025" cy="250032"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>319054</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="31" name="Arrow: Right 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D2168429-CDC0-4FFF-BCDC-285C06E8275B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="19053735">
+          <a:off x="1571625" y="6734175"/>
+          <a:ext cx="1852579" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:schemeClr val="accent5"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent5"/>
+        </a:fillRef>
+        <a:effectRef idx="3">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>85724</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>251896</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="32" name="Arrow: Right 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6AEAAD2F-78D8-43E6-A692-4728AB35C2D0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="1842930">
+          <a:off x="1847849" y="7791450"/>
+          <a:ext cx="1042472" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:schemeClr val="accent5"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent5"/>
+        </a:fillRef>
+        <a:effectRef idx="3">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>107157</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="34" name="Arrow: Right 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{93822A0E-CEA6-4DDE-883F-EB31FD65FF6E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6324600" y="8543925"/>
+          <a:ext cx="790575" cy="240507"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
           <a:avLst/>
@@ -1056,10 +1947,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:T15"/>
+  <dimension ref="B3:T51"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O44" sqref="O44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1077,23 +1968,25 @@
     <col min="12" max="12" width="12.28515625" style="1" customWidth="1"/>
     <col min="13" max="13" width="9.140625" style="1"/>
     <col min="14" max="14" width="6" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="1"/>
+    <col min="15" max="15" width="9.140625" style="1"/>
+    <col min="16" max="16" width="11.5703125" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:20" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="16" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="16"/>
-      <c r="H6" s="17" t="s">
+      <c r="D6" s="24"/>
+      <c r="H6" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="I6" s="17"/>
+      <c r="I6" s="25"/>
     </row>
     <row r="7" spans="2:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C7" s="14" t="s">
@@ -1119,10 +2012,10 @@
       <c r="G8" s="4"/>
       <c r="H8" s="11"/>
       <c r="I8" s="8"/>
-      <c r="K8" s="19" t="s">
+      <c r="K8" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="P8" s="19" t="s">
+      <c r="P8" s="17" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1131,11 +2024,11 @@
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
-      <c r="H9" s="17" t="s">
+      <c r="H9" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="I9" s="17"/>
-      <c r="K9" s="20">
+      <c r="I9" s="25"/>
+      <c r="K9" s="26">
         <f>D7*I7+D14*I14+I10</f>
         <v>7</v>
       </c>
@@ -1155,13 +2048,13 @@
       <c r="I10" s="10">
         <v>4</v>
       </c>
-      <c r="K10" s="21"/>
+      <c r="K10" s="27"/>
       <c r="P10" s="23"/>
-      <c r="R10" s="24" t="s">
+      <c r="R10" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="S10" s="25"/>
-      <c r="T10" s="25"/>
+      <c r="S10" s="21"/>
+      <c r="T10" s="21"/>
     </row>
     <row r="11" spans="2:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D11" s="6"/>
@@ -1170,7 +2063,7 @@
       <c r="G11" s="4"/>
       <c r="H11" s="11"/>
       <c r="I11" s="8"/>
-      <c r="K11" s="21"/>
+      <c r="K11" s="27"/>
       <c r="P11" s="23"/>
     </row>
     <row r="12" spans="2:20" ht="15.75" x14ac:dyDescent="0.25">
@@ -1182,17 +2075,17 @@
       <c r="I12" s="8"/>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="16"/>
+      <c r="D13" s="24"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
-      <c r="H13" s="17" t="s">
+      <c r="H13" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="I13" s="17"/>
+      <c r="I13" s="25"/>
     </row>
     <row r="14" spans="2:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C14" s="14" t="s">
@@ -1215,8 +2108,240 @@
       <c r="H15" s="11"/>
       <c r="I15" s="11"/>
     </row>
+    <row r="23" spans="2:20" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B23" s="16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="H25" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="I25" s="25"/>
+      <c r="J25" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="K25" s="25"/>
+    </row>
+    <row r="26" spans="2:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H26" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="I26" s="7">
+        <v>0</v>
+      </c>
+      <c r="J26" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="K26" s="13">
+        <v>1</v>
+      </c>
+      <c r="O26" s="17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="I27" s="28"/>
+      <c r="O27" s="22">
+        <f>1/(1-EXP(1)^(-J31))</f>
+        <v>1.0009127142532217</v>
+      </c>
+    </row>
+    <row r="28" spans="2:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D28" s="6"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="H28" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="I28" s="10">
+        <v>4</v>
+      </c>
+      <c r="O28" s="23"/>
+    </row>
+    <row r="29" spans="2:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D29" s="6"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="O29" s="23"/>
+    </row>
+    <row r="30" spans="2:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D30" s="6"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="J30" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="R30" s="20"/>
+      <c r="S30" s="21"/>
+      <c r="T30" s="21"/>
+    </row>
+    <row r="31" spans="2:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D31" s="6"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="26">
+        <f>D33*I26+D39*K26+I28</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="2:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C32" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="D32" s="24"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="8"/>
+      <c r="J32" s="27"/>
+    </row>
+    <row r="33" spans="3:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C33" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D33" s="15">
+        <v>2</v>
+      </c>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+      <c r="J33" s="27"/>
+    </row>
+    <row r="34" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+    </row>
+    <row r="35" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="H35" s="11"/>
+      <c r="I35" s="11"/>
+    </row>
+    <row r="38" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C38" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="D38" s="24"/>
+    </row>
+    <row r="39" spans="3:15" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="C39" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D39" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="H41" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="I41" s="25"/>
+      <c r="J41" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="K41" s="25"/>
+    </row>
+    <row r="42" spans="3:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H42" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="I42" s="7">
+        <v>0</v>
+      </c>
+      <c r="J42" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="K42" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
+      <c r="H43" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="I43" s="28"/>
+      <c r="O43" s="17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="3:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F44" s="4"/>
+      <c r="H44" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="I44" s="10">
+        <v>4</v>
+      </c>
+      <c r="O44" s="18"/>
+    </row>
+    <row r="45" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F45" s="4"/>
+      <c r="O45" s="19"/>
+    </row>
+    <row r="46" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F46" s="4"/>
+      <c r="G46" s="4"/>
+      <c r="J46" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="O46" s="19"/>
+    </row>
+    <row r="47" spans="3:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F47" s="4"/>
+      <c r="G47" s="4"/>
+      <c r="H47" s="11"/>
+      <c r="I47" s="8"/>
+      <c r="J47" s="26">
+        <f>D43*I42+D50*K42+I44</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="3:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F48" s="4"/>
+      <c r="G48" s="4"/>
+      <c r="H48" s="11"/>
+      <c r="I48" s="8"/>
+      <c r="J48" s="27"/>
+    </row>
+    <row r="49" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F49" s="4"/>
+      <c r="G49" s="4"/>
+      <c r="J49" s="27"/>
+    </row>
+    <row r="50" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F50" s="3"/>
+      <c r="G50" s="3"/>
+    </row>
+    <row r="51" spans="6:10" x14ac:dyDescent="0.2">
+      <c r="H51" s="11"/>
+      <c r="I51" s="11"/>
+    </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="18">
+    <mergeCell ref="J41:K41"/>
+    <mergeCell ref="H43:I43"/>
+    <mergeCell ref="J47:J49"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="J31:J33"/>
+    <mergeCell ref="O27:O29"/>
     <mergeCell ref="P9:P11"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="C13:D13"/>

</xml_diff>